<commit_message>
First set of comments addressed, missing basis oriented approach
</commit_message>
<xml_diff>
--- a/data/aggregated_single/bs1.xlsx
+++ b/data/aggregated_single/bs1.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12516" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12516" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="config" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="thermal" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="vres" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="hyd_storage" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="demand" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="cap_factors" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="config" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="thermal" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="vres" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="hyd_storage" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cap_factors" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="demand" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,13 +29,26 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color indexed="81"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.5999938962981048"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -50,9 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -444,7 +458,7 @@
           <t>periods</t>
         </is>
       </c>
-      <c r="B1" t="n">
+      <c r="B1" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -454,7 +468,7 @@
           <t>vc_nsp</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>5000</v>
       </c>
     </row>
@@ -472,10 +486,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col hidden="1" min="4" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -515,19 +532,19 @@
           <t>t1</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -545,7 +562,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -578,13 +595,13 @@
           <t>w1</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2" t="n">
         <v>3</v>
       </c>
     </row>
@@ -617,6 +634,55 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>generator</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>cap_factor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>w1</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -642,56 +708,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>207.8177326212711</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>period</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>generator</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>cap_factor</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>w1</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.6512451361867704</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>